<commit_message>
Added enemy stats display
</commit_message>
<xml_diff>
--- a/Assets/Excel/enemies.xlsx
+++ b/Assets/Excel/enemies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ulko\Assets\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{572D67A3-2EDA-4BCF-B894-D16979EF72FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D202E015-2D48-42D3-BE0D-9783C78F28B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4320" yWindow="3615" windowWidth="28800" windowHeight="15345" xr2:uid="{235337CE-ECDE-42A1-A64F-0EF6FACAA5A0}"/>
+    <workbookView xWindow="15315" yWindow="3780" windowWidth="17460" windowHeight="15345" xr2:uid="{235337CE-ECDE-42A1-A64F-0EF6FACAA5A0}"/>
   </bookViews>
   <sheets>
     <sheet name="enemies" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="18">
   <si>
     <t>id</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>sheet:intelligent_levels</t>
+  </si>
+  <si>
+    <t>maxHP</t>
   </si>
 </sst>
 </file>
@@ -458,7 +461,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -531,20 +534,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CF589C8-49E9-40E7-BF27-E18585058A4D}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="11.42578125" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -552,19 +555,22 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -572,16 +578,19 @@
         <v>0</v>
       </c>
       <c r="C2" s="2">
-        <f>50-D2-E2-F2</f>
         <v>30</v>
       </c>
       <c r="D2" s="2">
+        <f>50-E2-F2-G2</f>
+        <v>30</v>
+      </c>
+      <c r="E2" s="2">
         <v>5</v>
       </c>
-      <c r="E2" s="2">
+      <c r="F2" s="2">
         <v>10</v>
       </c>
-      <c r="F2" s="2">
+      <c r="G2" s="2">
         <v>5</v>
       </c>
     </row>
@@ -592,20 +601,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A18890BE-4E7E-4851-9CC8-CF6B4E45F9EF}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="11.42578125" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -613,19 +622,22 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -633,16 +645,19 @@
         <v>0</v>
       </c>
       <c r="C2" s="2">
-        <f>50-D2-E2-F2</f>
         <v>15</v>
       </c>
       <c r="D2" s="2">
+        <f>50-E2-F2-G2</f>
+        <v>15</v>
+      </c>
+      <c r="E2" s="2">
         <v>5</v>
       </c>
-      <c r="E2" s="2">
+      <c r="F2" s="2">
         <v>10</v>
       </c>
-      <c r="F2" s="2">
+      <c r="G2" s="2">
         <v>20</v>
       </c>
     </row>
@@ -653,20 +668,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC8AD53C-7693-4B88-B92B-A586F1339997}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="11.42578125" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -674,19 +689,22 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -694,16 +712,19 @@
         <v>0</v>
       </c>
       <c r="C2" s="2">
-        <f>50-D2-E2-F2</f>
         <v>15</v>
       </c>
       <c r="D2" s="2">
+        <f>50-E2-F2-G2</f>
+        <v>15</v>
+      </c>
+      <c r="E2" s="2">
         <v>20</v>
       </c>
-      <c r="E2" s="2">
+      <c r="F2" s="2">
         <v>5</v>
       </c>
-      <c r="F2" s="2">
+      <c r="G2" s="2">
         <v>10</v>
       </c>
     </row>
@@ -714,20 +735,20 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{999F2162-4F94-4C53-B229-8E98B7FC3215}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="11.42578125" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -735,19 +756,22 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -755,16 +779,19 @@
         <v>0</v>
       </c>
       <c r="C2" s="2">
-        <f>50-D2-E2-F2</f>
         <v>15</v>
       </c>
       <c r="D2" s="2">
+        <f>50-E2-F2-G2</f>
+        <v>15</v>
+      </c>
+      <c r="E2" s="2">
         <v>10</v>
       </c>
-      <c r="E2" s="2">
+      <c r="F2" s="2">
         <v>20</v>
       </c>
-      <c r="F2" s="2">
+      <c r="G2" s="2">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add strength to attacks
</commit_message>
<xml_diff>
--- a/Assets/Excel/enemies.xlsx
+++ b/Assets/Excel/enemies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ulko\Assets\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EED0945-8EE4-4CC7-B5FA-B14D7DD88247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9AF08E0-F0DC-47E1-BE08-6A41F9AE38DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{235337CE-ECDE-42A1-A64F-0EF6FACAA5A0}"/>
+    <workbookView xWindow="14100" yWindow="2910" windowWidth="19845" windowHeight="16785" activeTab="4" xr2:uid="{235337CE-ECDE-42A1-A64F-0EF6FACAA5A0}"/>
   </bookViews>
   <sheets>
     <sheet name="enemies" sheetId="1" r:id="rId1"/>
@@ -517,8 +517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CF589C8-49E9-40E7-BF27-E18585058A4D}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -607,7 +607,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -651,7 +651,7 @@
         <v>30</v>
       </c>
       <c r="D2" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E2" s="2">
         <v>0</v>
@@ -660,7 +660,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="2">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -674,7 +674,7 @@
         <v>60</v>
       </c>
       <c r="D3" s="2">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E3" s="2">
         <v>0</v>
@@ -683,7 +683,7 @@
         <v>0</v>
       </c>
       <c r="G3" s="2">
-        <v>40</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -696,7 +696,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -740,10 +740,10 @@
         <v>30</v>
       </c>
       <c r="D2" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E2" s="2">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F2" s="2">
         <v>0</v>
@@ -763,10 +763,10 @@
         <v>60</v>
       </c>
       <c r="D3" s="2">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E3" s="2">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="F3" s="2">
         <v>0</v>
@@ -784,8 +784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{999F2162-4F94-4C53-B229-8E98B7FC3215}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -829,13 +829,13 @@
         <v>30</v>
       </c>
       <c r="D2" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E2" s="2">
         <v>0</v>
       </c>
       <c r="F2" s="2">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="G2" s="2">
         <v>0</v>
@@ -852,13 +852,13 @@
         <v>60</v>
       </c>
       <c r="D3" s="2">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E3" s="2">
         <v>0</v>
       </c>
       <c r="F3" s="2">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="G3" s="2">
         <v>0</v>

</xml_diff>

<commit_message>
Added buff attack status
</commit_message>
<xml_diff>
--- a/Assets/Excel/enemies.xlsx
+++ b/Assets/Excel/enemies.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ulko\Assets\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9AE2B3A-4167-4C42-98D9-CE3A06CBE1F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B2EFEE1-BA2A-4BA8-9B6C-F0471D01073A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3120" yWindow="3120" windowWidth="28800" windowHeight="15150" activeTab="1" xr2:uid="{235337CE-ECDE-42A1-A64F-0EF6FACAA5A0}"/>
   </bookViews>
@@ -518,7 +518,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -562,7 +562,7 @@
         <v>30</v>
       </c>
       <c r="D2" s="2">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E2" s="2">
         <v>0</v>
@@ -585,7 +585,7 @@
         <v>80</v>
       </c>
       <c r="D3" s="2">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="E3" s="2">
         <v>0</v>

</xml_diff>

<commit_message>
Added first level placeholder
</commit_message>
<xml_diff>
--- a/Assets/Excel/enemies.xlsx
+++ b/Assets/Excel/enemies.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ulko\Assets\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5E9F14C-0F21-485D-88C1-1BC27ABE3DD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C48CD695-AB0A-45A7-B733-59313DC8D848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2010" yWindow="2040" windowWidth="33915" windowHeight="15150" activeTab="1" xr2:uid="{235337CE-ECDE-42A1-A64F-0EF6FACAA5A0}"/>
+    <workbookView xWindow="2010" yWindow="2040" windowWidth="33915" windowHeight="15150" activeTab="2" xr2:uid="{235337CE-ECDE-42A1-A64F-0EF6FACAA5A0}"/>
   </bookViews>
   <sheets>
     <sheet name="enemies" sheetId="1" r:id="rId1"/>
@@ -517,8 +517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CF589C8-49E9-40E7-BF27-E18585058A4D}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -559,7 +559,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="2">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="D2" s="2">
         <v>10</v>
@@ -606,8 +606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A18890BE-4E7E-4851-9CC8-CF6B4E45F9EF}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -648,10 +648,10 @@
         <v>8</v>
       </c>
       <c r="C2" s="2">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="D2" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E2" s="2">
         <v>0</v>

</xml_diff>

<commit_message>
Added witch boss battle
</commit_message>
<xml_diff>
--- a/Assets/Excel/enemies.xlsx
+++ b/Assets/Excel/enemies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ulko\Assets\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1DCA3EB-5649-42A5-969D-AF76D9187345}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{252E6018-1F1D-4760-A48E-611864ABD6B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2010" yWindow="2040" windowWidth="33915" windowHeight="15150" activeTab="3" xr2:uid="{235337CE-ECDE-42A1-A64F-0EF6FACAA5A0}"/>
+    <workbookView xWindow="630" yWindow="2655" windowWidth="33915" windowHeight="15150" activeTab="4" xr2:uid="{235337CE-ECDE-42A1-A64F-0EF6FACAA5A0}"/>
   </bookViews>
   <sheets>
     <sheet name="enemies" sheetId="1" r:id="rId1"/>
@@ -518,7 +518,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,10 +582,10 @@
         <v>16</v>
       </c>
       <c r="C3" s="2">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="D3" s="2">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E3" s="2">
         <v>0</v>
@@ -607,7 +607,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -671,10 +671,10 @@
         <v>16</v>
       </c>
       <c r="C3" s="2">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="D3" s="2">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E3" s="2">
         <v>0</v>
@@ -683,7 +683,7 @@
         <v>0</v>
       </c>
       <c r="G3" s="2">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -695,8 +695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC8AD53C-7693-4B88-B92B-A586F1339997}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -760,13 +760,13 @@
         <v>16</v>
       </c>
       <c r="C3" s="2">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="D3" s="2">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E3" s="2">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F3" s="2">
         <v>0</v>
@@ -784,8 +784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{999F2162-4F94-4C53-B229-8E98B7FC3215}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -849,16 +849,16 @@
         <v>16</v>
       </c>
       <c r="C3" s="2">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="D3" s="2">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E3" s="2">
         <v>0</v>
       </c>
       <c r="F3" s="2">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="G3" s="2">
         <v>0</v>

</xml_diff>

<commit_message>
Added the fields placeholder
</commit_message>
<xml_diff>
--- a/Assets/Excel/enemies.xlsx
+++ b/Assets/Excel/enemies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ulko\Assets\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B08490E3-562C-4047-A280-7AAE9CC88B4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B944B23-9B3C-4481-9FDC-6220DBFBD002}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="2655" windowWidth="33915" windowHeight="15150" activeTab="4" xr2:uid="{235337CE-ECDE-42A1-A64F-0EF6FACAA5A0}"/>
+    <workbookView xWindow="7590" yWindow="2820" windowWidth="33915" windowHeight="15150" activeTab="4" xr2:uid="{235337CE-ECDE-42A1-A64F-0EF6FACAA5A0}"/>
   </bookViews>
   <sheets>
     <sheet name="enemies" sheetId="1" r:id="rId1"/>
@@ -518,6 +518,95 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2">
+        <v>50</v>
+      </c>
+      <c r="D2" s="2">
+        <v>5</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2">
+        <v>150</v>
+      </c>
+      <c r="D3" s="2">
+        <v>25</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A18890BE-4E7E-4851-9CC8-CF6B4E45F9EF}">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
@@ -556,13 +645,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C2" s="2">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="D2" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E2" s="2">
         <v>0</v>
@@ -571,7 +660,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="2">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -579,13 +668,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="2">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C3" s="2">
-        <v>150</v>
+        <v>120</v>
       </c>
       <c r="D3" s="2">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="E3" s="2">
         <v>0</v>
@@ -594,7 +683,7 @@
         <v>0</v>
       </c>
       <c r="G3" s="2">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -602,12 +691,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A18890BE-4E7E-4851-9CC8-CF6B4E45F9EF}">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC8AD53C-7693-4B88-B92B-A586F1339997}">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -645,22 +734,22 @@
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C2" s="2">
         <v>60</v>
       </c>
       <c r="D2" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E2" s="2">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F2" s="2">
         <v>0</v>
       </c>
       <c r="G2" s="2">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -668,7 +757,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C3" s="2">
         <v>120</v>
@@ -677,13 +766,13 @@
         <v>10</v>
       </c>
       <c r="E3" s="2">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F3" s="2">
         <v>0</v>
       </c>
       <c r="G3" s="2">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -691,12 +780,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC8AD53C-7693-4B88-B92B-A586F1339997}">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{999F2162-4F94-4C53-B229-8E98B7FC3215}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -734,7 +823,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C2" s="2">
         <v>60</v>
@@ -743,10 +832,10 @@
         <v>5</v>
       </c>
       <c r="E2" s="2">
+        <v>0</v>
+      </c>
+      <c r="F2" s="2">
         <v>10</v>
-      </c>
-      <c r="F2" s="2">
-        <v>0</v>
       </c>
       <c r="G2" s="2">
         <v>0</v>
@@ -757,96 +846,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2">
-        <v>16</v>
-      </c>
-      <c r="C3" s="2">
-        <v>120</v>
-      </c>
-      <c r="D3" s="2">
-        <v>10</v>
-      </c>
-      <c r="E3" s="2">
-        <v>20</v>
-      </c>
-      <c r="F3" s="2">
-        <v>0</v>
-      </c>
-      <c r="G3" s="2">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{999F2162-4F94-4C53-B229-8E98B7FC3215}">
-  <dimension ref="A1:G3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="4" max="4" width="11.42578125" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2">
-        <v>2</v>
-      </c>
-      <c r="C2" s="2">
-        <v>60</v>
-      </c>
-      <c r="D2" s="2">
-        <v>5</v>
-      </c>
-      <c r="E2" s="2">
-        <v>0</v>
-      </c>
-      <c r="F2" s="2">
-        <v>10</v>
-      </c>
-      <c r="G2" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C3" s="2">
         <v>100</v>

</xml_diff>